<commit_message>
Statistics drafting in Koodit copy.xlsx
</commit_message>
<xml_diff>
--- a/Other_Notes/Koodit copy.xlsx
+++ b/Other_Notes/Koodit copy.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22220"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="1080" windowWidth="84700" windowHeight="62700" tabRatio="500"/>
+    <workbookView xWindow="16120" yWindow="10540" windowWidth="56480" windowHeight="29440" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Koodit copy.csv" sheetId="1" r:id="rId1"/>
+    <sheet name="Koodit" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1462" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="415">
   <si>
     <t>Category</t>
   </si>
@@ -1258,13 +1259,19 @@
   </si>
   <si>
     <t>Haastattelussa 5</t>
+  </si>
+  <si>
+    <t>Kategoriat</t>
+  </si>
+  <si>
+    <t>Alikategoriat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1288,6 +1295,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF454545"/>
+      <name val="Courier New"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1306,17 +1318,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1648,8 +1677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="F122" sqref="F122"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10014,6 +10043,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:E181">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color theme="3"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -10022,14 +10059,6 @@
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color theme="0"/>
-        <color theme="3"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
@@ -10044,4 +10073,801 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="B1" t="s">
+        <v>413</v>
+      </c>
+      <c r="D1" t="s">
+        <v>414</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>168</v>
+      </c>
+      <c r="K1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="17">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <f>COUNTIF(Koodit!F:F,A2)</f>
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <f>COUNTIF(Koodit!G:G,C2)</f>
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H2))</f>
+        <v>4</v>
+      </c>
+      <c r="J2" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H2))</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H2))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="17">
+      <c r="A3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3">
+        <f>COUNTIF(Koodit!F:F,A3)</f>
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <f>COUNTIF(Koodit!G:G,C3)</f>
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H3))</f>
+        <v>7</v>
+      </c>
+      <c r="J3" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H3))</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H3))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="17">
+      <c r="A4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B4">
+        <f>COUNTIF(Koodit!F:F,A4)</f>
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4">
+        <f>COUNTIF(Koodit!G:G,C4)</f>
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H4))</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H4))</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H4))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="17">
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5">
+        <f>COUNTIF(Koodit!G:G,C5)</f>
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H5))</f>
+        <v>4</v>
+      </c>
+      <c r="J5" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H5))</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H5))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="17">
+      <c r="C6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6">
+        <f>COUNTIF(Koodit!G:G,C6)</f>
+        <v>3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I6" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H6))</f>
+        <v>3</v>
+      </c>
+      <c r="J6" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H6))</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H6))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="17">
+      <c r="C7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7">
+        <f>COUNTIF(Koodit!G:G,C7)</f>
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>95</v>
+      </c>
+      <c r="I7" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H7))</f>
+        <v>6</v>
+      </c>
+      <c r="J7" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H7))</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H7))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="17">
+      <c r="C8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8">
+        <f>COUNTIF(Koodit!G:G,C8)</f>
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>114</v>
+      </c>
+      <c r="I8" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H8))</f>
+        <v>2</v>
+      </c>
+      <c r="J8" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H8))</f>
+        <v>26</v>
+      </c>
+      <c r="K8" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H8))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="17">
+      <c r="C9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9">
+        <f>COUNTIF(Koodit!G:G,C9)</f>
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>126</v>
+      </c>
+      <c r="I9" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H9))</f>
+        <v>2</v>
+      </c>
+      <c r="J9" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H9))</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H9))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="17">
+      <c r="C10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10">
+        <f>COUNTIF(Koodit!G:G,C10)</f>
+        <v>6</v>
+      </c>
+      <c r="H10" t="s">
+        <v>139</v>
+      </c>
+      <c r="I10" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H10))</f>
+        <v>1</v>
+      </c>
+      <c r="J10" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H10))</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H10))</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="17">
+      <c r="C11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11">
+        <f>COUNTIF(Koodit!G:G,C11)</f>
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>143</v>
+      </c>
+      <c r="I11" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H11))</f>
+        <v>3</v>
+      </c>
+      <c r="J11" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H11))</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H11))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="17">
+      <c r="C12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12">
+        <f>COUNTIF(Koodit!G:G,C12)</f>
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I12" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H12))</f>
+        <v>3</v>
+      </c>
+      <c r="J12" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H12))</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H12))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="17">
+      <c r="C13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D13">
+        <f>COUNTIF(Koodit!G:G,C13)</f>
+        <v>3</v>
+      </c>
+      <c r="H13" t="s">
+        <v>160</v>
+      </c>
+      <c r="I13" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H13))</f>
+        <v>3</v>
+      </c>
+      <c r="J13" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H13))</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H13))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="17">
+      <c r="C14" t="s">
+        <v>165</v>
+      </c>
+      <c r="D14">
+        <f>COUNTIF(Koodit!G:G,C14)</f>
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>165</v>
+      </c>
+      <c r="I14" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H14))</f>
+        <v>1</v>
+      </c>
+      <c r="J14" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H14))</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H14))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="17">
+      <c r="C15" t="s">
+        <v>169</v>
+      </c>
+      <c r="D15">
+        <f>COUNTIF(Koodit!G:G,C15)</f>
+        <v>5</v>
+      </c>
+      <c r="H15" t="s">
+        <v>169</v>
+      </c>
+      <c r="I15" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H15))</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H15))</f>
+        <v>5</v>
+      </c>
+      <c r="K15" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H15))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="17">
+      <c r="C16" t="s">
+        <v>181</v>
+      </c>
+      <c r="D16">
+        <f>COUNTIF(Koodit!G:G,C16)</f>
+        <v>6</v>
+      </c>
+      <c r="H16" t="s">
+        <v>181</v>
+      </c>
+      <c r="I16" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H16))</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H16))</f>
+        <v>6</v>
+      </c>
+      <c r="K16" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H16))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" ht="17">
+      <c r="C17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D17">
+        <f>COUNTIF(Koodit!G:G,C17)</f>
+        <v>3</v>
+      </c>
+      <c r="H17" t="s">
+        <v>196</v>
+      </c>
+      <c r="I17" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H17))</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H17))</f>
+        <v>3</v>
+      </c>
+      <c r="K17" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H17))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" ht="17">
+      <c r="C18" t="s">
+        <v>213</v>
+      </c>
+      <c r="D18">
+        <f>COUNTIF(Koodit!G:G,C18)</f>
+        <v>9</v>
+      </c>
+      <c r="H18" t="s">
+        <v>213</v>
+      </c>
+      <c r="I18" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H18))</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H18))</f>
+        <v>9</v>
+      </c>
+      <c r="K18" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H18))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" ht="17">
+      <c r="C19" t="s">
+        <v>237</v>
+      </c>
+      <c r="D19">
+        <f>COUNTIF(Koodit!G:G,C19)</f>
+        <v>5</v>
+      </c>
+      <c r="H19" t="s">
+        <v>237</v>
+      </c>
+      <c r="I19" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H19))</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H19))</f>
+        <v>5</v>
+      </c>
+      <c r="K19" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H19))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" ht="17">
+      <c r="C20" t="s">
+        <v>251</v>
+      </c>
+      <c r="D20">
+        <f>COUNTIF(Koodit!G:G,C20)</f>
+        <v>6</v>
+      </c>
+      <c r="H20" t="s">
+        <v>251</v>
+      </c>
+      <c r="I20" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H20))</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H20))</f>
+        <v>6</v>
+      </c>
+      <c r="K20" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H20))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" ht="17">
+      <c r="C21" t="s">
+        <v>300</v>
+      </c>
+      <c r="D21">
+        <f>COUNTIF(Koodit!G:G,C21)</f>
+        <v>10</v>
+      </c>
+      <c r="H21" t="s">
+        <v>300</v>
+      </c>
+      <c r="I21" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H21))</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H21))</f>
+        <v>10</v>
+      </c>
+      <c r="K21" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H21))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" ht="17">
+      <c r="C22" t="s">
+        <v>313</v>
+      </c>
+      <c r="D22">
+        <f>COUNTIF(Koodit!G:G,C22)</f>
+        <v>9</v>
+      </c>
+      <c r="H22" t="s">
+        <v>313</v>
+      </c>
+      <c r="I22" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H22))</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H22))</f>
+        <v>9</v>
+      </c>
+      <c r="K22" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H22))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" ht="17">
+      <c r="C23" t="s">
+        <v>326</v>
+      </c>
+      <c r="D23">
+        <f>COUNTIF(Koodit!G:G,C23)</f>
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>326</v>
+      </c>
+      <c r="I23" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H23))</f>
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H23))</f>
+        <v>1</v>
+      </c>
+      <c r="K23" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H23))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" ht="17">
+      <c r="C24" t="s">
+        <v>332</v>
+      </c>
+      <c r="D24">
+        <f>COUNTIF(Koodit!G:G,C24)</f>
+        <v>2</v>
+      </c>
+      <c r="H24" t="s">
+        <v>332</v>
+      </c>
+      <c r="I24" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H24))</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H24))</f>
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H24))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" ht="17">
+      <c r="C25" t="s">
+        <v>335</v>
+      </c>
+      <c r="D25">
+        <f>COUNTIF(Koodit!G:G,C25)</f>
+        <v>4</v>
+      </c>
+      <c r="H25" t="s">
+        <v>335</v>
+      </c>
+      <c r="I25" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H25))</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H25))</f>
+        <v>0</v>
+      </c>
+      <c r="K25" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H25))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" ht="17">
+      <c r="C26" t="s">
+        <v>341</v>
+      </c>
+      <c r="D26">
+        <f>COUNTIF(Koodit!G:G,C26)</f>
+        <v>13</v>
+      </c>
+      <c r="H26" t="s">
+        <v>341</v>
+      </c>
+      <c r="I26" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H26))</f>
+        <v>0</v>
+      </c>
+      <c r="J26" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H26))</f>
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H26))</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" ht="17">
+      <c r="C27" t="s">
+        <v>360</v>
+      </c>
+      <c r="D27">
+        <f>COUNTIF(Koodit!G:G,C27)</f>
+        <v>14</v>
+      </c>
+      <c r="H27" t="s">
+        <v>360</v>
+      </c>
+      <c r="I27" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H27))</f>
+        <v>0</v>
+      </c>
+      <c r="J27" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H27))</f>
+        <v>0</v>
+      </c>
+      <c r="K27" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H27))</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" ht="17">
+      <c r="C28" t="s">
+        <v>376</v>
+      </c>
+      <c r="D28">
+        <f>COUNTIF(Koodit!G:G,C28)</f>
+        <v>4</v>
+      </c>
+      <c r="H28" t="s">
+        <v>376</v>
+      </c>
+      <c r="I28" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H28))</f>
+        <v>0</v>
+      </c>
+      <c r="J28" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H28))</f>
+        <v>0</v>
+      </c>
+      <c r="K28" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H28))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" ht="17">
+      <c r="C29" t="s">
+        <v>382</v>
+      </c>
+      <c r="D29">
+        <f>COUNTIF(Koodit!G:G,C29)</f>
+        <v>4</v>
+      </c>
+      <c r="H29" t="s">
+        <v>382</v>
+      </c>
+      <c r="I29" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H29))</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H29))</f>
+        <v>0</v>
+      </c>
+      <c r="K29" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H29))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" ht="17">
+      <c r="C30" t="s">
+        <v>393</v>
+      </c>
+      <c r="D30">
+        <f>COUNTIF(Koodit!G:G,C30)</f>
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
+        <v>393</v>
+      </c>
+      <c r="I30" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H30))</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H30))</f>
+        <v>0</v>
+      </c>
+      <c r="K30" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H30))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" ht="17">
+      <c r="C31" t="s">
+        <v>396</v>
+      </c>
+      <c r="D31">
+        <f>COUNTIF(Koodit!G:G,C31)</f>
+        <v>10</v>
+      </c>
+      <c r="H31" t="s">
+        <v>396</v>
+      </c>
+      <c r="I31" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!I$1,Koodit!$G:$G,Sheet1!$H31))</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!J$1,Koodit!$G:$G,Sheet1!$H31))</f>
+        <v>0</v>
+      </c>
+      <c r="K31" s="1">
+        <f>SUM(COUNTIFS(Koodit!$F:$F,Sheet1!K$1,Koodit!$G:$G,Sheet1!$H31))</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="I2:K31">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="0"/>
+        <color theme="3"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>